<commit_message>
Several new improvements to processing and reporting
</commit_message>
<xml_diff>
--- a/QueryPerformance.xlsx
+++ b/QueryPerformance.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\XELoader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A74169D-5EF3-4897-AE54-0995C6578DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04981F9A-083A-4771-AA48-33F07281DBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B24106EA-52C9-4BFF-AE52-91EFFBA0713A}"/>
   </bookViews>
   <sheets>
-    <sheet name="AllProcDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="AllProcSummary" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="ReviewProcDetails" sheetId="5" r:id="rId3"/>
-    <sheet name="ReviewProcSummary" sheetId="6" state="hidden" r:id="rId4"/>
+    <sheet name="AllBatchDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="AllBatchSummary" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="ReviewBatchDetails" sheetId="5" r:id="rId3"/>
+    <sheet name="ReviewBatchSummary" sheetId="6" state="hidden" r:id="rId4"/>
     <sheet name="Charts" sheetId="3" r:id="rId5"/>
     <sheet name="DurationStats" sheetId="7" r:id="rId6"/>
     <sheet name="CPUStats" sheetId="8" r:id="rId7"/>
@@ -27,8 +27,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="619" r:id="rId12"/>
-    <pivotCache cacheId="624" r:id="rId13"/>
+    <pivotCache cacheId="714" r:id="rId12"/>
+    <pivotCache cacheId="720" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,12 +50,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>datetime</t>
-  </si>
-  <si>
-    <t>proc_name</t>
   </si>
   <si>
     <t>execution_count</t>
@@ -286,7 +283,13 @@
     <t>(blank)</t>
   </si>
   <si>
-    <t>NormText</t>
+    <t>database_name</t>
+  </si>
+  <si>
+    <t>(blank) Total</t>
+  </si>
+  <si>
+    <t>norm_text</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
     </dxf>
@@ -371,7 +380,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[QueryPerformance.xlsx]AllProcSummary!PivotTable1</c:name>
+    <c:name>[QueryPerformance.xlsx]AllBatchSummary!PivotTable1</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -646,7 +655,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AllProcSummary!$B$1</c:f>
+              <c:f>AllBatchSummary!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -669,7 +678,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>AllProcSummary!$A$2:$A$3</c:f>
+              <c:f>AllBatchSummary!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -680,7 +689,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AllProcSummary!$B$2:$B$3</c:f>
+              <c:f>AllBatchSummary!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -926,40 +935,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[QueryPerformance.xlsx]ReviewProcSummary!PivotTable3</c:name>
+    <c:name>[QueryPerformance.xlsx]ReviewBatchSummary!PivotTable3</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
@@ -3258,6 +3237,492 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="41"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="42"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="43"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="44"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="45"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="46"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="47"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="48"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="49"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="50"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="51"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="52"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="53"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="54"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="55"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="56"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="57"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="58"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -3269,11 +3734,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ReviewProcSummary!$B$1:$B$2</c:f>
+              <c:f>ReviewBatchSummary!$B$1:$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>(blank)</c:v>
+                  <c:v>(blank) - (blank)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3282,14 +3747,14 @@
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>ReviewProcSummary!$A$3:$A$4</c:f>
+              <c:f>ReviewBatchSummary!$A$4:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3300,7 +3765,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ReviewProcSummary!$B$3:$B$4</c:f>
+              <c:f>ReviewBatchSummary!$B$4:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -4698,17 +5163,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45498.61681053241" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{7AC009E6-F9F3-4083-894A-B72E2FB76FFE}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45499.581460300928" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{7AC009E6-F9F3-4083-894A-B72E2FB76FFE}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="10">
+  <cacheFields count="11">
     <cacheField name="datetime" numFmtId="164">
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-05-08T00:00:00" maxDate="2024-07-25T10:59:00" count="2971">
         <m/>
-        <d v="2024-07-25T10:12:00" u="1"/>
-        <d v="2024-07-25T10:13:00" u="1"/>
-        <d v="2024-07-25T10:14:00" u="1"/>
         <d v="2024-07-25T10:15:00" u="1"/>
         <d v="2024-07-25T10:16:00" u="1"/>
         <d v="2024-07-25T10:17:00" u="1"/>
@@ -4754,6 +5216,9 @@
         <d v="2024-07-25T10:57:00" u="1"/>
         <d v="2024-07-25T10:58:00" u="1"/>
         <d v="2024-07-25T10:59:00" u="1"/>
+        <d v="2024-07-25T10:12:00" u="1"/>
+        <d v="2024-07-25T10:13:00" u="1"/>
+        <d v="2024-07-25T10:14:00" u="1"/>
         <d v="2024-07-15T23:00:00" u="1"/>
         <d v="2024-07-15T23:01:00" u="1"/>
         <d v="2024-07-15T23:02:00" u="1"/>
@@ -7678,7 +8143,10 @@
         <d v="2024-05-08T23:41:00" u="1"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="proc_name" numFmtId="0">
+    <cacheField name="database_name" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="norm_text" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="execution_count" numFmtId="0">
@@ -7715,14 +8183,59 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45498.616810995372" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{BCC07ABF-141E-4A95-B7A4-936B2336CC3F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45499.581460763889" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{BCC07ABF-141E-4A95-B7A4-936B2336CC3F}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
-  <cacheFields count="10">
+  <cacheFields count="11">
     <cacheField name="datetime" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-05-08T00:00:00" maxDate="2024-07-16T22:57:00" count="2403">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-05-08T00:00:00" maxDate="2024-07-25T10:59:00" count="2448">
         <m/>
+        <d v="2024-07-25T10:15:00" u="1"/>
+        <d v="2024-07-25T10:16:00" u="1"/>
+        <d v="2024-07-25T10:17:00" u="1"/>
+        <d v="2024-07-25T10:18:00" u="1"/>
+        <d v="2024-07-25T10:19:00" u="1"/>
+        <d v="2024-07-25T10:20:00" u="1"/>
+        <d v="2024-07-25T10:21:00" u="1"/>
+        <d v="2024-07-25T10:22:00" u="1"/>
+        <d v="2024-07-25T10:23:00" u="1"/>
+        <d v="2024-07-25T10:24:00" u="1"/>
+        <d v="2024-07-25T10:25:00" u="1"/>
+        <d v="2024-07-25T10:26:00" u="1"/>
+        <d v="2024-07-25T10:27:00" u="1"/>
+        <d v="2024-07-25T10:28:00" u="1"/>
+        <d v="2024-07-25T10:29:00" u="1"/>
+        <d v="2024-07-25T10:30:00" u="1"/>
+        <d v="2024-07-25T10:31:00" u="1"/>
+        <d v="2024-07-25T10:32:00" u="1"/>
+        <d v="2024-07-25T10:33:00" u="1"/>
+        <d v="2024-07-25T10:34:00" u="1"/>
+        <d v="2024-07-25T10:35:00" u="1"/>
+        <d v="2024-07-25T10:36:00" u="1"/>
+        <d v="2024-07-25T10:37:00" u="1"/>
+        <d v="2024-07-25T10:38:00" u="1"/>
+        <d v="2024-07-25T10:39:00" u="1"/>
+        <d v="2024-07-25T10:40:00" u="1"/>
+        <d v="2024-07-25T10:41:00" u="1"/>
+        <d v="2024-07-25T10:42:00" u="1"/>
+        <d v="2024-07-25T10:43:00" u="1"/>
+        <d v="2024-07-25T10:44:00" u="1"/>
+        <d v="2024-07-25T10:45:00" u="1"/>
+        <d v="2024-07-25T10:46:00" u="1"/>
+        <d v="2024-07-25T10:47:00" u="1"/>
+        <d v="2024-07-25T10:48:00" u="1"/>
+        <d v="2024-07-25T10:49:00" u="1"/>
+        <d v="2024-07-25T10:50:00" u="1"/>
+        <d v="2024-07-25T10:51:00" u="1"/>
+        <d v="2024-07-25T10:52:00" u="1"/>
+        <d v="2024-07-25T10:53:00" u="1"/>
+        <d v="2024-07-25T10:54:00" u="1"/>
+        <d v="2024-07-25T10:55:00" u="1"/>
+        <d v="2024-07-25T10:56:00" u="1"/>
+        <d v="2024-07-25T10:57:00" u="1"/>
+        <d v="2024-07-25T10:58:00" u="1"/>
+        <d v="2024-07-25T10:59:00" u="1"/>
         <d v="2024-07-15T23:01:00" u="1"/>
         <d v="2024-07-15T23:03:00" u="1"/>
         <d v="2024-07-15T23:04:00" u="1"/>
@@ -10127,25 +10640,15 @@
         <d v="2024-05-08T23:41:00" u="1"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="proc_name" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="17">
+    <cacheField name="database_name" numFmtId="164">
+      <sharedItems containsNonDate="0" containsBlank="1" count="2">
         <m/>
-        <s v="GetAgencyPayPeriodCountsForDashboardView-20240424" u="1"/>
-        <s v="GetAgencyEmployerPensionSummaries-20240605" u="1"/>
-        <s v="GetMessagesForPayPeriod-20240424" u="1"/>
-        <s v="GetAgencyPayPeriodCountsForPeriodView-20240425" u="1"/>
-        <s v="GetMessagesForRecipient-20240424" u="1"/>
-        <s v="GetTeamMemberInformation-20240424" u="1"/>
-        <s v="GetAgencyPayPeriodCountsForSettingsView-20240424" u="1"/>
-        <s v="GetAgencyPayPeriodCountsForRunPayrollView-20240425" u="1"/>
-        <s v="GetUserProfilesForAgency-20240517" u="1"/>
-        <s v="GetMessages102" u="1"/>
-        <s v="GetAgencyPayPeriodCounts169" u="1"/>
-        <s v="GetAgencyPayPeriodCountsMinimum169" u="1"/>
-        <s v="GetAgencyEmployerPensionSummaries98" u="1"/>
-        <s v="GetPayPeriodCountsNano169" u="1"/>
-        <s v="GetTeamMemberInformation169" u="1"/>
-        <s v="GetUserProfilesForAgency" u="1"/>
+        <s v="PeopleWeb" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="norm_text" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="execution_count" numFmtId="0">
@@ -10194,6 +10697,7 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -10201,6 +10705,7 @@
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <m/>
@@ -10216,9 +10721,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ED96754-C7D7-4A08-AC1B-7D4287B3EA00}" name="PivotTable1" cacheId="619" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ED96754-C7D7-4A08-AC1B-7D4287B3EA00}" name="PivotTable1" cacheId="714" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
+  <pivotFields count="11">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="2972">
         <item m="1" x="1549"/>
@@ -13143,7 +13648,9 @@
         <item m="1" x="1486"/>
         <item m="1" x="1487"/>
         <item m="1" x="1488"/>
-        <item x="0"/>
+        <item m="1" x="46"/>
+        <item m="1" x="47"/>
+        <item m="1" x="48"/>
         <item m="1" x="1"/>
         <item m="1" x="2"/>
         <item m="1" x="3"/>
@@ -13189,12 +13696,11 @@
         <item m="1" x="43"/>
         <item m="1" x="44"/>
         <item m="1" x="45"/>
-        <item m="1" x="46"/>
-        <item m="1" x="47"/>
-        <item m="1" x="48"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -13210,7 +13716,7 @@
   </rowFields>
   <rowItems count="2">
     <i>
-      <x v="2922"/>
+      <x v="2970"/>
     </i>
     <i t="grand">
       <x/>
@@ -13220,7 +13726,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of cpu_pct" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of cpu_pct" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="2" format="2" series="1">
@@ -13246,56 +13752,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68B17D1C-59AA-4BF3-88FC-7EF3BD28DCA1}" name="PivotTable3" cacheId="624" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68B17D1C-59AA-4BF3-88FC-7EF3BD28DCA1}" name="PivotTable3" cacheId="720" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="A1:D5" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="11">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
-      <items count="2404">
-        <item m="1" x="1190"/>
-        <item m="1" x="1191"/>
-        <item m="1" x="1192"/>
-        <item m="1" x="1193"/>
-        <item m="1" x="1194"/>
-        <item m="1" x="1195"/>
-        <item m="1" x="1196"/>
-        <item m="1" x="1197"/>
-        <item m="1" x="1198"/>
-        <item m="1" x="1199"/>
-        <item m="1" x="1200"/>
-        <item m="1" x="1201"/>
-        <item m="1" x="1202"/>
-        <item m="1" x="1203"/>
-        <item m="1" x="1204"/>
-        <item m="1" x="1205"/>
-        <item m="1" x="1206"/>
-        <item m="1" x="1207"/>
-        <item m="1" x="1208"/>
-        <item m="1" x="1209"/>
-        <item m="1" x="1210"/>
-        <item m="1" x="1211"/>
-        <item m="1" x="1212"/>
-        <item m="1" x="1213"/>
-        <item m="1" x="1214"/>
-        <item m="1" x="1215"/>
-        <item m="1" x="1216"/>
-        <item m="1" x="1217"/>
-        <item m="1" x="1218"/>
-        <item m="1" x="1219"/>
-        <item m="1" x="1220"/>
-        <item m="1" x="1221"/>
-        <item m="1" x="1222"/>
-        <item m="1" x="1223"/>
-        <item m="1" x="1224"/>
-        <item m="1" x="1225"/>
-        <item m="1" x="1226"/>
-        <item m="1" x="1227"/>
-        <item m="1" x="1228"/>
-        <item m="1" x="1229"/>
-        <item m="1" x="1230"/>
-        <item m="1" x="1231"/>
-        <item m="1" x="1232"/>
-        <item m="1" x="1233"/>
-        <item m="1" x="1234"/>
+      <items count="2449">
         <item m="1" x="1235"/>
         <item m="1" x="1236"/>
         <item m="1" x="1237"/>
@@ -14464,51 +14925,51 @@
         <item m="1" x="2400"/>
         <item m="1" x="2401"/>
         <item m="1" x="2402"/>
-        <item m="1" x="1130"/>
-        <item m="1" x="1131"/>
-        <item m="1" x="1132"/>
-        <item m="1" x="1133"/>
-        <item m="1" x="1134"/>
-        <item m="1" x="1135"/>
-        <item m="1" x="1136"/>
-        <item m="1" x="1137"/>
-        <item m="1" x="1138"/>
-        <item m="1" x="1139"/>
-        <item m="1" x="1140"/>
-        <item m="1" x="1141"/>
-        <item m="1" x="1142"/>
-        <item m="1" x="1143"/>
-        <item m="1" x="1144"/>
-        <item m="1" x="1145"/>
-        <item m="1" x="1146"/>
-        <item m="1" x="1147"/>
-        <item m="1" x="1148"/>
-        <item m="1" x="1149"/>
-        <item m="1" x="1150"/>
-        <item m="1" x="1151"/>
-        <item m="1" x="1152"/>
-        <item m="1" x="1153"/>
-        <item m="1" x="1154"/>
-        <item m="1" x="1155"/>
-        <item m="1" x="1156"/>
-        <item m="1" x="1157"/>
-        <item m="1" x="1158"/>
-        <item m="1" x="1159"/>
-        <item m="1" x="1160"/>
-        <item m="1" x="1161"/>
-        <item m="1" x="1162"/>
-        <item m="1" x="1163"/>
-        <item m="1" x="1164"/>
-        <item m="1" x="1165"/>
-        <item m="1" x="1166"/>
-        <item m="1" x="1167"/>
-        <item m="1" x="1168"/>
-        <item m="1" x="1169"/>
-        <item m="1" x="1170"/>
-        <item m="1" x="1171"/>
-        <item m="1" x="1172"/>
-        <item m="1" x="1173"/>
-        <item m="1" x="1174"/>
+        <item m="1" x="2403"/>
+        <item m="1" x="2404"/>
+        <item m="1" x="2405"/>
+        <item m="1" x="2406"/>
+        <item m="1" x="2407"/>
+        <item m="1" x="2408"/>
+        <item m="1" x="2409"/>
+        <item m="1" x="2410"/>
+        <item m="1" x="2411"/>
+        <item m="1" x="2412"/>
+        <item m="1" x="2413"/>
+        <item m="1" x="2414"/>
+        <item m="1" x="2415"/>
+        <item m="1" x="2416"/>
+        <item m="1" x="2417"/>
+        <item m="1" x="2418"/>
+        <item m="1" x="2419"/>
+        <item m="1" x="2420"/>
+        <item m="1" x="2421"/>
+        <item m="1" x="2422"/>
+        <item m="1" x="2423"/>
+        <item m="1" x="2424"/>
+        <item m="1" x="2425"/>
+        <item m="1" x="2426"/>
+        <item m="1" x="2427"/>
+        <item m="1" x="2428"/>
+        <item m="1" x="2429"/>
+        <item m="1" x="2430"/>
+        <item m="1" x="2431"/>
+        <item m="1" x="2432"/>
+        <item m="1" x="2433"/>
+        <item m="1" x="2434"/>
+        <item m="1" x="2435"/>
+        <item m="1" x="2436"/>
+        <item m="1" x="2437"/>
+        <item m="1" x="2438"/>
+        <item m="1" x="2439"/>
+        <item m="1" x="2440"/>
+        <item m="1" x="2441"/>
+        <item m="1" x="2442"/>
+        <item m="1" x="2443"/>
+        <item m="1" x="2444"/>
+        <item m="1" x="2445"/>
+        <item m="1" x="2446"/>
+        <item m="1" x="2447"/>
         <item m="1" x="1175"/>
         <item m="1" x="1176"/>
         <item m="1" x="1177"/>
@@ -14524,51 +14985,51 @@
         <item m="1" x="1187"/>
         <item m="1" x="1188"/>
         <item m="1" x="1189"/>
-        <item m="1" x="1"/>
-        <item m="1" x="2"/>
-        <item m="1" x="3"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
-        <item m="1" x="8"/>
-        <item m="1" x="9"/>
-        <item m="1" x="10"/>
-        <item m="1" x="11"/>
-        <item m="1" x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item m="1" x="15"/>
-        <item m="1" x="16"/>
-        <item m="1" x="17"/>
-        <item m="1" x="18"/>
-        <item m="1" x="19"/>
-        <item m="1" x="20"/>
-        <item m="1" x="21"/>
-        <item m="1" x="22"/>
-        <item m="1" x="23"/>
-        <item m="1" x="24"/>
-        <item m="1" x="25"/>
-        <item m="1" x="26"/>
-        <item m="1" x="27"/>
-        <item m="1" x="28"/>
-        <item m="1" x="29"/>
-        <item m="1" x="30"/>
-        <item m="1" x="31"/>
-        <item m="1" x="32"/>
-        <item m="1" x="33"/>
-        <item m="1" x="34"/>
-        <item m="1" x="35"/>
-        <item m="1" x="36"/>
-        <item m="1" x="37"/>
-        <item m="1" x="38"/>
-        <item m="1" x="39"/>
-        <item m="1" x="40"/>
-        <item m="1" x="41"/>
-        <item m="1" x="42"/>
-        <item m="1" x="43"/>
-        <item m="1" x="44"/>
-        <item m="1" x="45"/>
+        <item m="1" x="1190"/>
+        <item m="1" x="1191"/>
+        <item m="1" x="1192"/>
+        <item m="1" x="1193"/>
+        <item m="1" x="1194"/>
+        <item m="1" x="1195"/>
+        <item m="1" x="1196"/>
+        <item m="1" x="1197"/>
+        <item m="1" x="1198"/>
+        <item m="1" x="1199"/>
+        <item m="1" x="1200"/>
+        <item m="1" x="1201"/>
+        <item m="1" x="1202"/>
+        <item m="1" x="1203"/>
+        <item m="1" x="1204"/>
+        <item m="1" x="1205"/>
+        <item m="1" x="1206"/>
+        <item m="1" x="1207"/>
+        <item m="1" x="1208"/>
+        <item m="1" x="1209"/>
+        <item m="1" x="1210"/>
+        <item m="1" x="1211"/>
+        <item m="1" x="1212"/>
+        <item m="1" x="1213"/>
+        <item m="1" x="1214"/>
+        <item m="1" x="1215"/>
+        <item m="1" x="1216"/>
+        <item m="1" x="1217"/>
+        <item m="1" x="1218"/>
+        <item m="1" x="1219"/>
+        <item m="1" x="1220"/>
+        <item m="1" x="1221"/>
+        <item m="1" x="1222"/>
+        <item m="1" x="1223"/>
+        <item m="1" x="1224"/>
+        <item m="1" x="1225"/>
+        <item m="1" x="1226"/>
+        <item m="1" x="1227"/>
+        <item m="1" x="1228"/>
+        <item m="1" x="1229"/>
+        <item m="1" x="1230"/>
+        <item m="1" x="1231"/>
+        <item m="1" x="1232"/>
+        <item m="1" x="1233"/>
+        <item m="1" x="1234"/>
         <item m="1" x="46"/>
         <item m="1" x="47"/>
         <item m="1" x="48"/>
@@ -15653,28 +16114,109 @@
         <item m="1" x="1127"/>
         <item m="1" x="1128"/>
         <item m="1" x="1129"/>
+        <item m="1" x="1130"/>
+        <item m="1" x="1131"/>
+        <item m="1" x="1132"/>
+        <item m="1" x="1133"/>
+        <item m="1" x="1134"/>
+        <item m="1" x="1135"/>
+        <item m="1" x="1136"/>
+        <item m="1" x="1137"/>
+        <item m="1" x="1138"/>
+        <item m="1" x="1139"/>
+        <item m="1" x="1140"/>
+        <item m="1" x="1141"/>
+        <item m="1" x="1142"/>
+        <item m="1" x="1143"/>
+        <item m="1" x="1144"/>
+        <item m="1" x="1145"/>
+        <item m="1" x="1146"/>
+        <item m="1" x="1147"/>
+        <item m="1" x="1148"/>
+        <item m="1" x="1149"/>
+        <item m="1" x="1150"/>
+        <item m="1" x="1151"/>
+        <item m="1" x="1152"/>
+        <item m="1" x="1153"/>
+        <item m="1" x="1154"/>
+        <item m="1" x="1155"/>
+        <item m="1" x="1156"/>
+        <item m="1" x="1157"/>
+        <item m="1" x="1158"/>
+        <item m="1" x="1159"/>
+        <item m="1" x="1160"/>
+        <item m="1" x="1161"/>
+        <item m="1" x="1162"/>
+        <item m="1" x="1163"/>
+        <item m="1" x="1164"/>
+        <item m="1" x="1165"/>
+        <item m="1" x="1166"/>
+        <item m="1" x="1167"/>
+        <item m="1" x="1168"/>
+        <item m="1" x="1169"/>
+        <item m="1" x="1170"/>
+        <item m="1" x="1171"/>
+        <item m="1" x="1172"/>
+        <item m="1" x="1173"/>
+        <item m="1" x="1174"/>
+        <item m="1" x="1"/>
+        <item m="1" x="2"/>
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item m="1" x="6"/>
+        <item m="1" x="7"/>
+        <item m="1" x="8"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item m="1" x="11"/>
+        <item m="1" x="12"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item m="1" x="15"/>
+        <item m="1" x="16"/>
+        <item m="1" x="17"/>
+        <item m="1" x="18"/>
+        <item m="1" x="19"/>
+        <item m="1" x="20"/>
+        <item m="1" x="21"/>
+        <item m="1" x="22"/>
+        <item m="1" x="23"/>
+        <item m="1" x="24"/>
+        <item m="1" x="25"/>
+        <item m="1" x="26"/>
+        <item m="1" x="27"/>
+        <item m="1" x="28"/>
+        <item m="1" x="29"/>
+        <item m="1" x="30"/>
+        <item m="1" x="31"/>
+        <item m="1" x="32"/>
+        <item m="1" x="33"/>
+        <item m="1" x="34"/>
+        <item m="1" x="35"/>
+        <item m="1" x="36"/>
+        <item m="1" x="37"/>
+        <item m="1" x="38"/>
+        <item m="1" x="39"/>
+        <item m="1" x="40"/>
+        <item m="1" x="41"/>
+        <item m="1" x="42"/>
+        <item m="1" x="43"/>
+        <item m="1" x="44"/>
+        <item m="1" x="45"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="18">
-        <item m="1" x="13"/>
-        <item m="1" x="11"/>
-        <item m="1" x="12"/>
-        <item m="1" x="10"/>
-        <item m="1" x="14"/>
-        <item m="1" x="15"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="4"/>
+      <items count="3">
         <item m="1" x="1"/>
-        <item m="1" x="7"/>
-        <item m="1" x="5"/>
-        <item m="1" x="3"/>
-        <item m="1" x="6"/>
-        <item m="1" x="2"/>
-        <item m="1" x="9"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
@@ -15693,152 +16235,37 @@
   </rowFields>
   <rowItems count="2">
     <i>
-      <x v="2402"/>
+      <x v="2447"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
+  <colFields count="2">
     <field x="1"/>
+    <field x="2"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="3">
     <i>
-      <x v="16"/>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default">
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of cpu_pct" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of cpu_pct" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="11">
+  <chartFormats count="1">
     <chartFormat chart="2" format="30" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="31" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="32" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="33" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="34" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="35" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="36" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="37" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="38" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="15"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="39" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="40" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="16"/>
           </reference>
         </references>
       </pivotArea>
@@ -15857,11 +16284,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}" name="Table1" displayName="Table1" ref="A1:J2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{69F8F33B-4158-43F5-8204-07D90F01E0EB}" name="datetime" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{17C5FD6B-772D-4EBD-9816-3AAE3664FDF1}" name="proc_name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}" name="Table1" displayName="Table1" ref="A1:K2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:K2" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{69F8F33B-4158-43F5-8204-07D90F01E0EB}" name="datetime" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{51278D32-7C3B-4B59-86DF-7A4B462EB9E9}" name="database_name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{17C5FD6B-772D-4EBD-9816-3AAE3664FDF1}" name="norm_text"/>
     <tableColumn id="3" xr3:uid="{FD3209D6-279F-4A1C-9506-31B9340FD95C}" name="execution_count"/>
     <tableColumn id="4" xr3:uid="{018236F7-AE50-48B1-8F1D-3F620BEB0519}" name="duration_microseconds"/>
     <tableColumn id="5" xr3:uid="{F26D22C1-98F0-496E-A034-163FED3EB541}" name="cpu_microseconds"/>
@@ -15876,11 +16304,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}" name="Table2" displayName="Table2" ref="A1:J2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{C9936654-3AC7-4718-9342-9EC0D1ECFFD6}" name="datetime" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{E3EBBBE3-5710-4030-AA38-E20AD4553B08}" name="proc_name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}" name="Table2" displayName="Table2" ref="A1:K2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:K2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{C9936654-3AC7-4718-9342-9EC0D1ECFFD6}" name="datetime" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{9963A2D7-7F0A-4494-8E13-E2961DC8EAD5}" name="database_name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E3EBBBE3-5710-4030-AA38-E20AD4553B08}" name="norm_text"/>
     <tableColumn id="3" xr3:uid="{171E3D44-C982-47E6-9CFA-6053A5502BA0}" name="execution_count"/>
     <tableColumn id="4" xr3:uid="{082936FB-CE75-4AF1-9141-A3AA9A819EC3}" name="duration_microseconds"/>
     <tableColumn id="5" xr3:uid="{2FA61231-D12A-4CD5-8A9C-080E918E7020}" name="cpu_microseconds"/>
@@ -15895,10 +16324,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}" name="Table3" displayName="Table3" ref="A1:L2" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9F89287D-53BA-40B5-A5EE-FB681DD6B95F}" name="NormText"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}" name="Table3" displayName="Table3" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}"/>
+  <tableColumns count="13">
+    <tableColumn id="13" xr3:uid="{C2CCC2BD-37A2-45E4-ACAB-0C81405E1697}" name="database_name"/>
+    <tableColumn id="1" xr3:uid="{9F89287D-53BA-40B5-A5EE-FB681DD6B95F}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{ADE2F75D-0AFE-4B1D-8B44-D7C6EE9B28E3}" name="execution_count"/>
     <tableColumn id="3" xr3:uid="{98F9E5BB-3A19-42B7-AA92-2669C9E73486}" name="min_duration"/>
     <tableColumn id="4" xr3:uid="{1FAA5B7E-1AD7-43A8-BFB5-E4AA98594E96}" name="mean_duration"/>
@@ -15916,10 +16346,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{23EB7B8E-749A-41A7-995D-960631E8F9CE}" name="Table3511" displayName="Table3511" ref="A1:L2" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{A1FD3BC7-8B0B-4BD0-8E6C-092A384E08E4}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{01ABADDB-7A04-4D3C-9F67-D2B0D5740743}" name="NormText"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{23EB7B8E-749A-41A7-995D-960631E8F9CE}" name="Table3511" displayName="Table3511" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{A1FD3BC7-8B0B-4BD0-8E6C-092A384E08E4}"/>
+  <tableColumns count="13">
+    <tableColumn id="3" xr3:uid="{3CC2CD8A-004A-4290-937E-EF08FA9CB80B}" name="database_name"/>
+    <tableColumn id="1" xr3:uid="{01ABADDB-7A04-4D3C-9F67-D2B0D5740743}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{E0E9F6EA-D31C-4249-B92D-A8A19924C2F6}" name="execution_count"/>
     <tableColumn id="13" xr3:uid="{F9F1FF0D-8907-43DB-9E0B-4BC23B3DB014}" name="min_cpu_time"/>
     <tableColumn id="14" xr3:uid="{D3A51BD5-6632-4423-A3B6-84758343286B}" name="mean_cpu_time"/>
@@ -15937,10 +16368,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{93BEC30A-09F1-4FEE-97F0-47B6427FBD5E}" name="Table361218" displayName="Table361218" ref="A1:L2" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{174DD456-9DE2-4F9C-B4AE-612141D59BB0}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{7ACB1737-DC9F-4D99-BC7F-881593DC8172}" name="NormText"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{93BEC30A-09F1-4FEE-97F0-47B6427FBD5E}" name="Table361218" displayName="Table361218" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{174DD456-9DE2-4F9C-B4AE-612141D59BB0}"/>
+  <tableColumns count="13">
+    <tableColumn id="3" xr3:uid="{DD1227E5-1935-40AD-B23B-09578193531F}" name="database_name"/>
+    <tableColumn id="1" xr3:uid="{7ACB1737-DC9F-4D99-BC7F-881593DC8172}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{7D95A36B-F8C1-4453-9CD9-01A486DF1C53}" name="execution_count"/>
     <tableColumn id="23" xr3:uid="{AB439EA2-F8AE-4E28-9A0C-C15EBBABA478}" name="min_logical_reads"/>
     <tableColumn id="24" xr3:uid="{90AC7838-4F7E-40E7-86C7-819AA594745A}" name="mean_logical_reads"/>
@@ -15958,10 +16390,11 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{F0068F5C-7E1A-4797-A0AB-EC2906576BE4}" name="Table37131925" displayName="Table37131925" ref="A1:L2" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{332B5612-12BE-481C-842C-353F69027BA8}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D7AF0615-D8F9-4E88-BD61-5DFFB69A59E9}" name="NormText"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{F0068F5C-7E1A-4797-A0AB-EC2906576BE4}" name="Table37131925" displayName="Table37131925" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{332B5612-12BE-481C-842C-353F69027BA8}"/>
+  <tableColumns count="13">
+    <tableColumn id="3" xr3:uid="{89165832-E568-4B1C-B848-89303B8115AB}" name="database_name"/>
+    <tableColumn id="1" xr3:uid="{D7AF0615-D8F9-4E88-BD61-5DFFB69A59E9}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{377D8477-4782-4361-A45E-DB348740D2E8}" name="execution_count"/>
     <tableColumn id="33" xr3:uid="{2B9A7491-9CC1-4C5F-B12F-626D91EA2EEA}" name="min_physical_reads"/>
     <tableColumn id="34" xr3:uid="{9D2629A5-5686-41BA-BA83-3A9B3F7A4118}" name="mean_physical_reads"/>
@@ -15979,10 +16412,11 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{17257BAF-5D37-4780-B03D-AE18CDD9FB34}" name="Table3814202632" displayName="Table3814202632" ref="A1:L2" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{0BF94567-BB14-4990-B412-EE1EFDA0F11A}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{C92D9531-D954-4B54-9F8E-9CEBF1B1AAB5}" name="NormText"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{17257BAF-5D37-4780-B03D-AE18CDD9FB34}" name="Table3814202632" displayName="Table3814202632" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{0BF94567-BB14-4990-B412-EE1EFDA0F11A}"/>
+  <tableColumns count="13">
+    <tableColumn id="3" xr3:uid="{699DFBDF-8080-46A4-9748-818B1F406FC1}" name="database_name"/>
+    <tableColumn id="1" xr3:uid="{C92D9531-D954-4B54-9F8E-9CEBF1B1AAB5}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{1365AF57-FCDE-4CA0-BBB4-32B2FFF73881}" name="execution_count"/>
     <tableColumn id="43" xr3:uid="{7089C0A2-49B9-4936-B7C1-7C9AF72ACD37}" name="min_writes"/>
     <tableColumn id="44" xr3:uid="{6CBB548A-9C6F-47E9-A1B2-4F07D1944ECF}" name="mean_writes"/>
@@ -16000,10 +16434,11 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{01FD9972-1522-4AE0-924C-47A16C3F31A4}" name="Table391521273339" displayName="Table391521273339" ref="A1:L2" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{4547EA9B-8543-48D2-B17D-7794DE8A6E16}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{3954441D-135E-4FE2-AB68-8FF413CB516E}" name="NormText"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{01FD9972-1522-4AE0-924C-47A16C3F31A4}" name="Table391521273339" displayName="Table391521273339" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{4547EA9B-8543-48D2-B17D-7794DE8A6E16}"/>
+  <tableColumns count="13">
+    <tableColumn id="3" xr3:uid="{6B13C351-B984-4814-AACF-D33AEC9625F2}" name="database_name"/>
+    <tableColumn id="1" xr3:uid="{3954441D-135E-4FE2-AB68-8FF413CB516E}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{2BE0C866-C963-4119-AA9F-A725F1384B5D}" name="execution_count"/>
     <tableColumn id="53" xr3:uid="{F6DA99E8-55AB-4B5D-930C-0EF02C454A34}" name="min_row_count"/>
     <tableColumn id="54" xr3:uid="{A1AD5065-7603-4D03-8E8C-0DB3988823F1}" name="mean_row_count"/>
@@ -16337,7 +16772,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9506BB-2498-4EA9-91C6-C9697376216C}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -16346,47 +16781,51 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="71.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -16399,25 +16838,28 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00040C4-3078-44F7-B695-B3399B6FFAD3}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
@@ -16458,42 +16900,45 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>62</v>
-      </c>
-      <c r="L1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -16506,25 +16951,28 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F224642-2D58-4E64-9F68-674F0EB31D92}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="28" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
@@ -16565,42 +17013,45 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>71</v>
-      </c>
-      <c r="L1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -16616,32 +17067,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4"/>
     </row>
@@ -16652,7 +17104,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB83DB8-54CC-4858-8DC1-33FD57E1DFFC}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -16661,47 +17113,51 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="71.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -16714,57 +17170,80 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631114B7-7266-4DF3-84D2-8C5566EE20D7}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
+      <c r="B3" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16783,17 +17262,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -16804,25 +17283,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F347CCB-CBDE-44BF-B642-4C1E4055DDCA}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
@@ -16863,42 +17345,45 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -16911,25 +17396,28 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C97FAF-BC91-4BEC-AB56-3B61CB806F13}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
@@ -16970,42 +17458,45 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -17018,25 +17509,28 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F559BBA-3642-484C-91F4-EEEC18344FA4}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
@@ -17077,42 +17571,45 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>42</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -17125,25 +17622,28 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C7D1A4-77A4-445A-9DF8-DA8122B41740}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
@@ -17184,42 +17684,45 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>52</v>
-      </c>
-      <c r="L1" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Normalised text with Hex values not normalised.  Add NormTextHashId to QueryPerformance.xlsx and XELoaderQueries.sql
</commit_message>
<xml_diff>
--- a/QueryPerformance.xlsx
+++ b/QueryPerformance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\XELoader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04981F9A-083A-4771-AA48-33F07281DBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19AFA83-E1E3-485B-9CAC-118C79CEE06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B24106EA-52C9-4BFF-AE52-91EFFBA0713A}"/>
   </bookViews>
@@ -27,8 +27,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="714" r:id="rId12"/>
-    <pivotCache cacheId="720" r:id="rId13"/>
+    <pivotCache cacheId="774" r:id="rId12"/>
+    <pivotCache cacheId="781" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
   <si>
     <t>datetime</t>
   </si>
@@ -291,6 +291,9 @@
   <si>
     <t>norm_text</t>
   </si>
+  <si>
+    <t>norm_text_hash_id</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +343,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy\ hh:mm:ss"/>
     </dxf>
@@ -939,6 +948,36 @@
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
@@ -3723,6 +3762,62 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="59"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -3734,11 +3829,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ReviewBatchSummary!$B$1:$B$3</c:f>
+              <c:f>ReviewBatchSummary!$B$1:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>(blank) - (blank)</c:v>
+                  <c:v>(blank) - (blank) - (blank)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3747,14 +3842,14 @@
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln w="25400">
+            <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>ReviewBatchSummary!$A$4:$A$5</c:f>
+              <c:f>ReviewBatchSummary!$A$5:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3765,7 +3860,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ReviewBatchSummary!$B$4:$B$5</c:f>
+              <c:f>ReviewBatchSummary!$B$5:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -5087,13 +5182,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5125,13 +5220,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5163,11 +5258,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45499.581460300928" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{7AC009E6-F9F3-4083-894A-B72E2FB76FFE}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45503.441248263887" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{7AC009E6-F9F3-4083-894A-B72E2FB76FFE}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="11">
+  <cacheFields count="12">
     <cacheField name="datetime" numFmtId="164">
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-05-08T00:00:00" maxDate="2024-07-25T10:59:00" count="2971">
         <m/>
@@ -8143,6 +8238,9 @@
         <d v="2024-05-08T23:41:00" u="1"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="norm_text_hash_id" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
     <cacheField name="database_name" numFmtId="164">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -8183,11 +8281,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45499.581460763889" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{BCC07ABF-141E-4A95-B7A4-936B2336CC3F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Robert Horrocks" refreshedDate="45503.441248842595" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{BCC07ABF-141E-4A95-B7A4-936B2336CC3F}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
-  <cacheFields count="11">
+  <cacheFields count="12">
     <cacheField name="datetime" numFmtId="164">
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-05-08T00:00:00" maxDate="2024-07-25T10:59:00" count="2448">
         <m/>
@@ -10640,6 +10738,11 @@
         <d v="2024-05-08T23:41:00" u="1"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="norm_text_hash_id" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
     <cacheField name="database_name" numFmtId="164">
       <sharedItems containsNonDate="0" containsBlank="1" count="2">
         <m/>
@@ -10698,6 +10801,7 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -10705,6 +10809,7 @@
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
@@ -10721,9 +10826,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ED96754-C7D7-4A08-AC1B-7D4287B3EA00}" name="PivotTable1" cacheId="714" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ED96754-C7D7-4A08-AC1B-7D4287B3EA00}" name="PivotTable1" cacheId="774" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
+  <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="2972">
         <item m="1" x="1549"/>
@@ -13705,6 +13810,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -13726,7 +13832,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of cpu_pct" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of cpu_pct" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="2" format="2" series="1">
@@ -13752,9 +13858,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68B17D1C-59AA-4BF3-88FC-7EF3BD28DCA1}" name="PivotTable3" cacheId="720" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="A1:D5" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68B17D1C-59AA-4BF3-88FC-7EF3BD28DCA1}" name="PivotTable3" cacheId="781" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="A1:E6" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="2449">
         <item m="1" x="1235"/>
@@ -16209,6 +16315,12 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
       <items count="3">
         <item m="1" x="1"/>
         <item x="0"/>
@@ -16241,30 +16353,50 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="2">
+  <colFields count="3">
     <field x="1"/>
     <field x="2"/>
+    <field x="3"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
+      <x/>
       <x v="1"/>
       <x/>
     </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
     <i t="default">
-      <x v="1"/>
+      <x/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of cpu_pct" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of cpu_pct" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="2" format="30" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="59" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -16284,11 +16416,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}" name="Table1" displayName="Table1" ref="A1:K2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{69F8F33B-4158-43F5-8204-07D90F01E0EB}" name="datetime" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{51278D32-7C3B-4B59-86DF-7A4B462EB9E9}" name="database_name" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}" name="Table1" displayName="Table1" ref="A1:L2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:L2" xr:uid="{C7FA1B7E-C0DA-4D7A-AA35-375029784535}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{69F8F33B-4158-43F5-8204-07D90F01E0EB}" name="datetime" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{B58890FF-E583-4DBD-A2F5-9F589D2466B5}" name="norm_text_hash_id" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{51278D32-7C3B-4B59-86DF-7A4B462EB9E9}" name="database_name" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{17C5FD6B-772D-4EBD-9816-3AAE3664FDF1}" name="norm_text"/>
     <tableColumn id="3" xr3:uid="{FD3209D6-279F-4A1C-9506-31B9340FD95C}" name="execution_count"/>
     <tableColumn id="4" xr3:uid="{018236F7-AE50-48B1-8F1D-3F620BEB0519}" name="duration_microseconds"/>
@@ -16304,11 +16437,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}" name="Table2" displayName="Table2" ref="A1:K2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{C9936654-3AC7-4718-9342-9EC0D1ECFFD6}" name="datetime" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{9963A2D7-7F0A-4494-8E13-E2961DC8EAD5}" name="database_name" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}" name="Table2" displayName="Table2" ref="A1:L2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:L2" xr:uid="{A62E67F2-A94D-40D1-BC6C-D44992EFC38D}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{C9936654-3AC7-4718-9342-9EC0D1ECFFD6}" name="datetime" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{EEBAE9C0-0C27-4C31-A029-C5CDBD7FE1C5}" name="norm_text_hash_id" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{9963A2D7-7F0A-4494-8E13-E2961DC8EAD5}" name="database_name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{E3EBBBE3-5710-4030-AA38-E20AD4553B08}" name="norm_text"/>
     <tableColumn id="3" xr3:uid="{171E3D44-C982-47E6-9CFA-6053A5502BA0}" name="execution_count"/>
     <tableColumn id="4" xr3:uid="{082936FB-CE75-4AF1-9141-A3AA9A819EC3}" name="duration_microseconds"/>
@@ -16324,9 +16458,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}" name="Table3" displayName="Table3" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{DB1720B7-55CB-4433-8BB1-8A24DE0FAA46}"/>
+  <tableColumns count="14">
+    <tableColumn id="14" xr3:uid="{7C30B4D4-2B90-4AB7-8491-B1D3F256A847}" name="norm_text_hash_id"/>
     <tableColumn id="13" xr3:uid="{C2CCC2BD-37A2-45E4-ACAB-0C81405E1697}" name="database_name"/>
     <tableColumn id="1" xr3:uid="{9F89287D-53BA-40B5-A5EE-FB681DD6B95F}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{ADE2F75D-0AFE-4B1D-8B44-D7C6EE9B28E3}" name="execution_count"/>
@@ -16346,9 +16481,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{23EB7B8E-749A-41A7-995D-960631E8F9CE}" name="Table3511" displayName="Table3511" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{A1FD3BC7-8B0B-4BD0-8E6C-092A384E08E4}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{23EB7B8E-749A-41A7-995D-960631E8F9CE}" name="Table3511" displayName="Table3511" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{A1FD3BC7-8B0B-4BD0-8E6C-092A384E08E4}"/>
+  <tableColumns count="14">
+    <tableColumn id="4" xr3:uid="{50F77733-CFDF-4D86-B2DC-68B01A81A9A9}" name="norm_text_hash_id"/>
     <tableColumn id="3" xr3:uid="{3CC2CD8A-004A-4290-937E-EF08FA9CB80B}" name="database_name"/>
     <tableColumn id="1" xr3:uid="{01ABADDB-7A04-4D3C-9F67-D2B0D5740743}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{E0E9F6EA-D31C-4249-B92D-A8A19924C2F6}" name="execution_count"/>
@@ -16368,9 +16504,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{93BEC30A-09F1-4FEE-97F0-47B6427FBD5E}" name="Table361218" displayName="Table361218" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{174DD456-9DE2-4F9C-B4AE-612141D59BB0}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{93BEC30A-09F1-4FEE-97F0-47B6427FBD5E}" name="Table361218" displayName="Table361218" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{174DD456-9DE2-4F9C-B4AE-612141D59BB0}"/>
+  <tableColumns count="14">
+    <tableColumn id="4" xr3:uid="{79C1C2BD-7F08-42F5-9A11-9EB4BF3C059F}" name="norm_text_hash_id"/>
     <tableColumn id="3" xr3:uid="{DD1227E5-1935-40AD-B23B-09578193531F}" name="database_name"/>
     <tableColumn id="1" xr3:uid="{7ACB1737-DC9F-4D99-BC7F-881593DC8172}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{7D95A36B-F8C1-4453-9CD9-01A486DF1C53}" name="execution_count"/>
@@ -16390,9 +16527,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{F0068F5C-7E1A-4797-A0AB-EC2906576BE4}" name="Table37131925" displayName="Table37131925" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{332B5612-12BE-481C-842C-353F69027BA8}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{F0068F5C-7E1A-4797-A0AB-EC2906576BE4}" name="Table37131925" displayName="Table37131925" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{332B5612-12BE-481C-842C-353F69027BA8}"/>
+  <tableColumns count="14">
+    <tableColumn id="4" xr3:uid="{F1CD3BE9-5D34-4829-9FAD-C8126D2C138C}" name="norm_text_hash_id"/>
     <tableColumn id="3" xr3:uid="{89165832-E568-4B1C-B848-89303B8115AB}" name="database_name"/>
     <tableColumn id="1" xr3:uid="{D7AF0615-D8F9-4E88-BD61-5DFFB69A59E9}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{377D8477-4782-4361-A45E-DB348740D2E8}" name="execution_count"/>
@@ -16412,9 +16550,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{17257BAF-5D37-4780-B03D-AE18CDD9FB34}" name="Table3814202632" displayName="Table3814202632" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{0BF94567-BB14-4990-B412-EE1EFDA0F11A}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{17257BAF-5D37-4780-B03D-AE18CDD9FB34}" name="Table3814202632" displayName="Table3814202632" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{0BF94567-BB14-4990-B412-EE1EFDA0F11A}"/>
+  <tableColumns count="14">
+    <tableColumn id="4" xr3:uid="{783FA46B-7D1F-43D3-AD99-D577449EDA3D}" name="norm_text_hash_id"/>
     <tableColumn id="3" xr3:uid="{699DFBDF-8080-46A4-9748-818B1F406FC1}" name="database_name"/>
     <tableColumn id="1" xr3:uid="{C92D9531-D954-4B54-9F8E-9CEBF1B1AAB5}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{1365AF57-FCDE-4CA0-BBB4-32B2FFF73881}" name="execution_count"/>
@@ -16434,9 +16573,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{01FD9972-1522-4AE0-924C-47A16C3F31A4}" name="Table391521273339" displayName="Table391521273339" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{4547EA9B-8543-48D2-B17D-7794DE8A6E16}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{01FD9972-1522-4AE0-924C-47A16C3F31A4}" name="Table391521273339" displayName="Table391521273339" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{4547EA9B-8543-48D2-B17D-7794DE8A6E16}"/>
+  <tableColumns count="14">
+    <tableColumn id="4" xr3:uid="{C54D8228-E07B-40EC-A782-FA7B249AB8BF}" name="norm_text_hash_id"/>
     <tableColumn id="3" xr3:uid="{6B13C351-B984-4814-AACF-D33AEC9625F2}" name="database_name"/>
     <tableColumn id="1" xr3:uid="{3954441D-135E-4FE2-AB68-8FF413CB516E}" name="norm_text"/>
     <tableColumn id="2" xr3:uid="{2BE0C866-C963-4119-AA9F-A725F1384B5D}" name="execution_count"/>
@@ -16772,7 +16912,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9506BB-2498-4EA9-91C6-C9697376216C}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -16780,51 +16920,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="71.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -16838,7 +16981,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00040C4-3078-44F7-B695-B3399B6FFAD3}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -16900,44 +17043,47 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>60</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -16951,7 +17097,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F224642-2D58-4E64-9F68-674F0EB31D92}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -17013,44 +17159,47 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -17104,7 +17253,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB83DB8-54CC-4858-8DC1-33FD57E1DFFC}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -17112,51 +17261,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="71.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -17170,7 +17322,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631114B7-7266-4DF3-84D2-8C5566EE20D7}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -17180,9 +17332,8 @@
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
@@ -17202,7 +17353,7 @@
     <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -17210,40 +17361,50 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>76</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>76</v>
       </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17252,7 +17413,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CCB406-45EE-4FF1-B58B-FE788B02DE98}">
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -17265,13 +17426,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>75</v>
       </c>
     </row>
@@ -17283,7 +17444,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F347CCB-CBDE-44BF-B642-4C1E4055DDCA}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -17345,44 +17506,47 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -17396,7 +17560,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C97FAF-BC91-4BEC-AB56-3B61CB806F13}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -17458,44 +17622,47 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -17509,7 +17676,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F559BBA-3642-484C-91F4-EEEC18344FA4}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -17571,44 +17738,47 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -17622,7 +17792,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C7D1A4-77A4-445A-9DF8-DA8122B41740}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -17684,44 +17854,47 @@
     <col min="59" max="61" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Freeze Pains issue in QueryPerformance.xlsx
</commit_message>
<xml_diff>
--- a/QueryPerformance.xlsx
+++ b/QueryPerformance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\XELoader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484A4558-06A9-405D-ACA3-9D6DB98608C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85017F4C-F154-4121-B41E-D121A9C6251C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{B24106EA-52C9-4BFF-AE52-91EFFBA0713A}"/>
   </bookViews>
@@ -27,8 +27,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="872" r:id="rId12"/>
-    <pivotCache cacheId="876" r:id="rId13"/>
+    <pivotCache cacheId="955" r:id="rId12"/>
+    <pivotCache cacheId="956" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -331,14 +331,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2128,6 +2127,62 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="21"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -7301,7 +7356,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ED96754-C7D7-4A08-AC1B-7D4287B3EA00}" name="PivotTable1" cacheId="876" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ED96754-C7D7-4A08-AC1B-7D4287B3EA00}" name="PivotTable1" cacheId="956" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
@@ -10872,7 +10927,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3C35A375-7966-4646-8505-24ADEE604741}" name="PivotTable15" cacheId="872" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3C35A375-7966-4646-8505-24ADEE604741}" name="PivotTable15" cacheId="955" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
@@ -10963,7 +11018,7 @@
   <dataFields count="1">
     <dataField name="Sum of cpu_pct" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="7">
+  <chartFormats count="8">
     <chartFormat chart="2" format="14" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="4">
@@ -11086,6 +11141,24 @@
           </reference>
           <reference field="3" count="1" selected="0">
             <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
@@ -11602,8 +11675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9506BB-2498-4EA9-91C6-C9697376216C}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11927,13 +12000,11 @@
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12081,19 +12152,11 @@
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>